<commit_message>
added script for excel
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F658512D-CB1B-4AA7-93C3-A3A825DF9E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0441611-7918-4072-96BC-559B5ECAC6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="linear Interp" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="linear interp 2D" sheetId="3" r:id="rId3"/>
     <sheet name="pseudo random" sheetId="4" r:id="rId4"/>
     <sheet name="sobol random" sheetId="5" r:id="rId5"/>
+    <sheet name="script" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,6 +171,10 @@
     <t>sobol</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>call pays MAX(spot() - 120, 0.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -218,7 +223,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -233,6 +238,12 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -22142,7 +22153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68004832-4959-427C-BC92-94F61EF49DAC}">
   <dimension ref="A1:T211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -38604,4 +38615,134 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
+  <dimension ref="A2:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="106.75" customWidth="1"/>
+    <col min="2" max="3" width="58.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>45925</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="str" cm="1">
+        <f t="array" aca="1" ref="A4" ca="1">_xll.PRODUCT.NEW("ss",A2,B2)</f>
+        <v>~ScriptProduct~ss~00000196A0B6BA50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="str" cm="1">
+        <f t="array" aca="1" ref="A6:A21" ca="1">_xll.PRODUCT.DEBUG(A4)</f>
+        <v>Event: 1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f ca="1"/>
+        <v>Statement: 1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f ca="1"/>
+        <v>PAYS(</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve"> VAR[-1]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f ca="1"/>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve"> MAX(</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve">  MINUS(</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve">   SPOT</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve">  ,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve">   CONST[120.000000]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve">  )</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve"> ,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve">  CONST[0.000000]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f ca="1"/>
+        <v xml:space="preserve"> )</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f ca="1"/>
+        <v>)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added full examples of script product pricing
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEF39E0-4B70-43F8-A557-B2FF852FBA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6426B3D6-042B-4FA7-8E0E-C140D0D6BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -172,10 +172,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>call pays MAX(spot() - 120, 0.0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>spot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -189,6 +185,10 @@
   </si>
   <si>
     <t>div</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>call pays MAX(spot() - 120, 0.0)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -38635,10 +38635,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -38648,145 +38648,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+      <c r="A1" s="5">
+        <v>44829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" cm="1">
+        <f t="array" aca="1" ref="A2" ca="1">_xll.EVALUATIONDATE.SET(A1)</f>
+        <v>44829</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>45925</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="D1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>45925</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>29</v>
-      </c>
-      <c r="D2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="str" cm="1">
-        <f t="array" aca="1" ref="A4" ca="1">_xll.PRODUCT.NEW("ss",A2,B2)</f>
-        <v>~ScriptProduct~ss~00000196A0B6BA50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="str" cm="1">
-        <f t="array" aca="1" ref="A6:A21" ca="1">_xll.PRODUCT.DEBUG(A4)</f>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="str" cm="1">
+        <f t="array" aca="1" ref="A5" ca="1">_xll.PRODUCT.NEW("my_product",A3,B3)</f>
+        <v>~ScriptProduct~my_product~000001F78B4EAA60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="str" cm="1">
+        <f t="array" aca="1" ref="A7:A22" ca="1">_xll.PRODUCT.DEBUG(A5)</f>
         <v>Event: 1</v>
       </c>
-      <c r="C6" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xll.BSMODELDATA.NEW("model",D1,D2,D3,D4)</f>
-        <v>~BSModelData_~model~000002093EAA3110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
-        <f ca="1"/>
-        <v>Statement: 1</v>
+      <c r="C7" t="str" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">_xll.BSMODELDATA.NEW("model",D2,D3,D4,D5)</f>
+        <v>~BSModelData~model~000001F78446B820</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f ca="1"/>
-        <v>PAYS(</v>
+        <v>Statement: 1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f ca="1"/>
-        <v xml:space="preserve"> VAR[-1]</v>
+        <v>PAYS(</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f ca="1"/>
-        <v>,</v>
+        <v xml:space="preserve"> VAR[-1]</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f ca="1"/>
-        <v xml:space="preserve"> MAX(</v>
+        <v>,</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f ca="1"/>
-        <v xml:space="preserve">  MINUS(</v>
+        <v xml:space="preserve"> MAX(</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f ca="1"/>
-        <v xml:space="preserve">   SPOT</v>
+        <v xml:space="preserve">  MINUS(</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f ca="1"/>
-        <v xml:space="preserve">  ,</v>
+        <v xml:space="preserve">   SPOT</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f ca="1"/>
-        <v xml:space="preserve">   CONST[120.000000]</v>
+        <v xml:space="preserve">  ,</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f ca="1"/>
+        <v xml:space="preserve">   CONST[120.000000]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f ca="1"/>
         <v xml:space="preserve">  )</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
         <f ca="1"/>
         <v xml:space="preserve"> ,</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
         <f ca="1"/>
         <v xml:space="preserve">  CONST[0.000000]</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="str">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
         <f ca="1"/>
         <v xml:space="preserve"> )</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="str">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
         <f ca="1"/>
         <v>)</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="str">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
         <f ca="1"/>
         <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="str" cm="1">
+        <f t="array" aca="1" ref="A24:B24" ca="1">_xll.MONTECARLO.VALUE(A5,C7,2^20,"sobol",FALSE)</f>
+        <v>value</v>
+      </c>
+      <c r="B24" s="2">
+        <f ca="1"/>
+        <v>4.0389474364897877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update setup and readme
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6426B3D6-042B-4FA7-8E0E-C140D0D6BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36C976C-D838-4D28-9E54-F8D6966EF4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -38635,10 +38635,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -38689,7 +38689,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str" cm="1">
         <f t="array" aca="1" ref="A5" ca="1">_xll.PRODUCT.NEW("my_product",A3,B3)</f>
-        <v>~ScriptProduct~my_product~000001F78B4EAA60</v>
+        <v>~ScriptProduct~my_product~0000029A2FF687A0</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -38705,7 +38705,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.BSMODELDATA.NEW("model",D2,D3,D4,D5)</f>
-        <v>~BSModelData~model~000001F78446B820</v>
+        <v>~BSModelData~model~0000029A40A07900</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -38808,8 +38808,12 @@
         <v>4.0389474364897877</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
using aad in public example
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36C976C-D838-4D28-9E54-F8D6966EF4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B051F88-8E24-4E96-A315-1FE26E22DAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
@@ -38635,10 +38635,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -38689,7 +38689,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str" cm="1">
         <f t="array" aca="1" ref="A5" ca="1">_xll.PRODUCT.NEW("my_product",A3,B3)</f>
-        <v>~ScriptProduct~my_product~0000029A2FF687A0</v>
+        <v>~ScriptProduct~my_product~000001F00EF47480</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -38705,7 +38705,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.BSMODELDATA.NEW("model",D2,D3,D4,D5)</f>
-        <v>~BSModelData~model~0000029A40A07900</v>
+        <v>~BSModelData~model~000001F00F28DAF0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -38799,17 +38799,54 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="str" cm="1">
-        <f t="array" aca="1" ref="A24:B24" ca="1">_xll.MONTECARLO.VALUE(A5,C7,2^20,"sobol",FALSE)</f>
+      <c r="A24" t="str">
+        <f t="array" aca="1" ref="A24:B28" ca="1">_xll.MONTECARLO.VALUE(A5,C7,2^20,"sobol",FALSE,TRUE,0.01)</f>
+        <v>d_div</v>
+      </c>
+      <c r="B24" s="2">
+        <f ca="1"/>
+        <v>-85.228968760590448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f ca="1"/>
+        <v>d_rate</v>
+      </c>
+      <c r="B25">
+        <f ca="1"/>
+        <v>73.10106084118145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f ca="1"/>
+        <v>d_spot</v>
+      </c>
+      <c r="B26">
+        <f ca="1"/>
+        <v>0.28383735034320723</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f ca="1"/>
+        <v>d_vol</v>
+      </c>
+      <c r="B27" s="2">
+        <f ca="1"/>
+        <v>58.71397201095639</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f ca="1"/>
         <v>value</v>
       </c>
-      <c r="B24" s="2">
-        <f ca="1"/>
-        <v>4.0389474364897877</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="2"/>
+      <c r="B28">
+        <f ca="1"/>
+        <v>4.0389474366644285</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fixed uoc script product example
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B051F88-8E24-4E96-A315-1FE26E22DAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FEA874-BBC5-49F5-BA35-E84D73E70531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="37">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,25 @@
   </si>
   <si>
     <t>call pays MAX(spot() - 120, 0.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if spot() &gt; 150 then alive = 0 endif</t>
+  </si>
+  <si>
+    <t>if spot() &gt; 150 then alive = 0 endif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uoc pays alive * MAX(spot() - 120, 0.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alive = 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -38635,10 +38654,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -38688,8 +38707,8 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str" cm="1">
-        <f t="array" aca="1" ref="A5" ca="1">_xll.PRODUCT.NEW("my_product",A3,B3)</f>
-        <v>~ScriptProduct~my_product~000001F00EF47480</v>
+        <f t="array" aca="1" ref="A5" ca="1">_xll.PRODUCT.NEW("my_product",A31:A189,B31:B189)</f>
+        <v>~ScriptProduct~my_product~000002F2399736D0</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -38705,7 +38724,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.BSMODELDATA.NEW("model",D2,D3,D4,D5)</f>
-        <v>~BSModelData~model~000001F00F28DAF0</v>
+        <v>~BSModelData~model~000002F2269954B0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -38800,12 +38819,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f t="array" aca="1" ref="A24:B28" ca="1">_xll.MONTECARLO.VALUE(A5,C7,2^20,"sobol",FALSE,TRUE,0.01)</f>
+        <f t="array" aca="1" ref="A24:B28" ca="1">_xll.MONTECARLO.VALUE(A5,C7,2^20,"sobol",FALSE,TRUE,0.1)</f>
         <v>d_div</v>
       </c>
       <c r="B24" s="2">
         <f ca="1"/>
-        <v>-85.228968760590448</v>
+        <v>-45.307943019269025</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -38815,7 +38834,7 @@
       </c>
       <c r="B25">
         <f ca="1"/>
-        <v>73.10106084118145</v>
+        <v>41.948712910691313</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -38825,7 +38844,7 @@
       </c>
       <c r="B26">
         <f ca="1"/>
-        <v>0.28383735034320723</v>
+        <v>0.15088867885066817</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -38835,7 +38854,7 @@
       </c>
       <c r="B27" s="2">
         <f ca="1"/>
-        <v>58.71397201095639</v>
+        <v>22.83584680328406</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -38845,7 +38864,1284 @@
       </c>
       <c r="B28">
         <f ca="1"/>
-        <v>4.0389474366644285</v>
+        <v>1.1187217058675882</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>44829</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>44836</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>44843</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>44850</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>44857</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>44864</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>44871</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>44878</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>44892</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>44899</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>44906</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>44913</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>44920</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>44927</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>44934</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>44941</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>44948</v>
+      </c>
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>44955</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>44962</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>44969</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>44976</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>44983</v>
+      </c>
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>44990</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>44997</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>45004</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>45011</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>45018</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>45025</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>45032</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>45039</v>
+      </c>
+      <c r="B61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>45046</v>
+      </c>
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
+        <v>45053</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>45060</v>
+      </c>
+      <c r="B64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>45067</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>45074</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>45081</v>
+      </c>
+      <c r="B67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>45088</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>45095</v>
+      </c>
+      <c r="B69" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>45102</v>
+      </c>
+      <c r="B70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>45109</v>
+      </c>
+      <c r="B71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>45116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
+        <v>45123</v>
+      </c>
+      <c r="B73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>45130</v>
+      </c>
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="5">
+        <v>45137</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
+        <v>45144</v>
+      </c>
+      <c r="B76" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="5">
+        <v>45151</v>
+      </c>
+      <c r="B77" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="5">
+        <v>45158</v>
+      </c>
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="5">
+        <v>45165</v>
+      </c>
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="5">
+        <v>45172</v>
+      </c>
+      <c r="B80" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="5">
+        <v>45179</v>
+      </c>
+      <c r="B81" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="5">
+        <v>45186</v>
+      </c>
+      <c r="B82" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="5">
+        <v>45193</v>
+      </c>
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
+        <v>45200</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="5">
+        <v>45207</v>
+      </c>
+      <c r="B85" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>45214</v>
+      </c>
+      <c r="B86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="5">
+        <v>45221</v>
+      </c>
+      <c r="B87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>45228</v>
+      </c>
+      <c r="B88" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
+        <v>45235</v>
+      </c>
+      <c r="B89" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>45242</v>
+      </c>
+      <c r="B90" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>45249</v>
+      </c>
+      <c r="B91" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>45256</v>
+      </c>
+      <c r="B92" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="5">
+        <v>45263</v>
+      </c>
+      <c r="B93" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
+        <v>45270</v>
+      </c>
+      <c r="B94" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="5">
+        <v>45277</v>
+      </c>
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="5">
+        <v>45284</v>
+      </c>
+      <c r="B96" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="5">
+        <v>45291</v>
+      </c>
+      <c r="B97" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="5">
+        <v>45298</v>
+      </c>
+      <c r="B98" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="5">
+        <v>45305</v>
+      </c>
+      <c r="B99" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="5">
+        <v>45312</v>
+      </c>
+      <c r="B100" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="5">
+        <v>45319</v>
+      </c>
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="5">
+        <v>45326</v>
+      </c>
+      <c r="B102" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="5">
+        <v>45333</v>
+      </c>
+      <c r="B103" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="5">
+        <v>45340</v>
+      </c>
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="5">
+        <v>45347</v>
+      </c>
+      <c r="B105" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="5">
+        <v>45354</v>
+      </c>
+      <c r="B106" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="5">
+        <v>45361</v>
+      </c>
+      <c r="B107" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="5">
+        <v>45368</v>
+      </c>
+      <c r="B108" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="5">
+        <v>45375</v>
+      </c>
+      <c r="B109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="5">
+        <v>45382</v>
+      </c>
+      <c r="B110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="5">
+        <v>45389</v>
+      </c>
+      <c r="B111" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="5">
+        <v>45396</v>
+      </c>
+      <c r="B112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="5">
+        <v>45403</v>
+      </c>
+      <c r="B113" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="5">
+        <v>45410</v>
+      </c>
+      <c r="B114" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="5">
+        <v>45417</v>
+      </c>
+      <c r="B115" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="5">
+        <v>45424</v>
+      </c>
+      <c r="B116" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="5">
+        <v>45431</v>
+      </c>
+      <c r="B117" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="5">
+        <v>45438</v>
+      </c>
+      <c r="B118" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="5">
+        <v>45445</v>
+      </c>
+      <c r="B119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="5">
+        <v>45452</v>
+      </c>
+      <c r="B120" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="5">
+        <v>45459</v>
+      </c>
+      <c r="B121" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="5">
+        <v>45466</v>
+      </c>
+      <c r="B122" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="5">
+        <v>45473</v>
+      </c>
+      <c r="B123" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="5">
+        <v>45480</v>
+      </c>
+      <c r="B124" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="5">
+        <v>45487</v>
+      </c>
+      <c r="B125" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="5">
+        <v>45494</v>
+      </c>
+      <c r="B126" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B127" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="5">
+        <v>45508</v>
+      </c>
+      <c r="B128" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="5">
+        <v>45515</v>
+      </c>
+      <c r="B129" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="5">
+        <v>45522</v>
+      </c>
+      <c r="B130" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="5">
+        <v>45529</v>
+      </c>
+      <c r="B131" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B132" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="5">
+        <v>45543</v>
+      </c>
+      <c r="B133" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="5">
+        <v>45550</v>
+      </c>
+      <c r="B134" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="5">
+        <v>45557</v>
+      </c>
+      <c r="B135" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="5">
+        <v>45564</v>
+      </c>
+      <c r="B136" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="5">
+        <v>45571</v>
+      </c>
+      <c r="B137" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="5">
+        <v>45578</v>
+      </c>
+      <c r="B138" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="5">
+        <v>45585</v>
+      </c>
+      <c r="B139" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="5">
+        <v>45592</v>
+      </c>
+      <c r="B140" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="5">
+        <v>45599</v>
+      </c>
+      <c r="B141" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="5">
+        <v>45606</v>
+      </c>
+      <c r="B142" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="5">
+        <v>45613</v>
+      </c>
+      <c r="B143" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="5">
+        <v>45620</v>
+      </c>
+      <c r="B144" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="5">
+        <v>45627</v>
+      </c>
+      <c r="B145" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="5">
+        <v>45634</v>
+      </c>
+      <c r="B146" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="5">
+        <v>45641</v>
+      </c>
+      <c r="B147" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="5">
+        <v>45648</v>
+      </c>
+      <c r="B148" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="5">
+        <v>45655</v>
+      </c>
+      <c r="B149" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="5">
+        <v>45662</v>
+      </c>
+      <c r="B150" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="5">
+        <v>45669</v>
+      </c>
+      <c r="B151" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="5">
+        <v>45676</v>
+      </c>
+      <c r="B152" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="5">
+        <v>45683</v>
+      </c>
+      <c r="B153" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="5">
+        <v>45690</v>
+      </c>
+      <c r="B154" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="5">
+        <v>45697</v>
+      </c>
+      <c r="B155" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="5">
+        <v>45704</v>
+      </c>
+      <c r="B156" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="5">
+        <v>45711</v>
+      </c>
+      <c r="B157" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="5">
+        <v>45718</v>
+      </c>
+      <c r="B158" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="5">
+        <v>45725</v>
+      </c>
+      <c r="B159" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="5">
+        <v>45732</v>
+      </c>
+      <c r="B160" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="5">
+        <v>45739</v>
+      </c>
+      <c r="B161" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="5">
+        <v>45746</v>
+      </c>
+      <c r="B162" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="5">
+        <v>45753</v>
+      </c>
+      <c r="B163" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="5">
+        <v>45760</v>
+      </c>
+      <c r="B164" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="5">
+        <v>45767</v>
+      </c>
+      <c r="B165" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="5">
+        <v>45774</v>
+      </c>
+      <c r="B166" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="5">
+        <v>45781</v>
+      </c>
+      <c r="B167" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="5">
+        <v>45788</v>
+      </c>
+      <c r="B168" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="5">
+        <v>45795</v>
+      </c>
+      <c r="B169" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="5">
+        <v>45802</v>
+      </c>
+      <c r="B170" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="5">
+        <v>45809</v>
+      </c>
+      <c r="B171" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="5">
+        <v>45816</v>
+      </c>
+      <c r="B172" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="5">
+        <v>45823</v>
+      </c>
+      <c r="B173" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="5">
+        <v>45830</v>
+      </c>
+      <c r="B174" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="5">
+        <v>45837</v>
+      </c>
+      <c r="B175" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="5">
+        <v>45844</v>
+      </c>
+      <c r="B176" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="5">
+        <v>45851</v>
+      </c>
+      <c r="B177" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="5">
+        <v>45858</v>
+      </c>
+      <c r="B178" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="5">
+        <v>45865</v>
+      </c>
+      <c r="B179" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="5">
+        <v>45872</v>
+      </c>
+      <c r="B180" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="5">
+        <v>45879</v>
+      </c>
+      <c r="B181" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="5">
+        <v>45886</v>
+      </c>
+      <c r="B182" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="5">
+        <v>45893</v>
+      </c>
+      <c r="B183" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="5">
+        <v>45900</v>
+      </c>
+      <c r="B184" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="5">
+        <v>45907</v>
+      </c>
+      <c r="B185" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="5">
+        <v>45914</v>
+      </c>
+      <c r="B186" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="5">
+        <v>45921</v>
+      </c>
+      <c r="B187" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="5">
+        <v>45925</v>
+      </c>
+      <c r="B188" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="5">
+        <v>45925</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some screen shot
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECC63EF-41AF-4C07-BB7C-AB377D2AEF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEEA140-105D-48CA-86F2-8C0F485B96A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="9165" windowWidth="25245" windowHeight="11835" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="linear Interp" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -38707,8 +38707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
   <dimension ref="A1:D2869"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
remove reposity in python
</commit_message>
<xml_diff>
--- a/excel/dal 101.xlsx
+++ b/excel/dal 101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451AB528-3EEC-439F-BA86-8569D0C648D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCDE99D-1AA7-49CA-930A-BD0FA5601506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,6 +213,14 @@
   </si>
   <si>
     <t>Model Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repository size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repository model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -38702,10 +38710,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F20376B-A517-4185-B924-84028E73DAC7}">
-  <dimension ref="A1:D2871"/>
+  <dimension ref="A1:H2871"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -38714,10 +38722,13 @@
     <col min="2" max="2" width="77.625" style="6" customWidth="1"/>
     <col min="3" max="3" width="58.75" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="6"/>
+    <col min="5" max="5" width="9" style="6"/>
+    <col min="6" max="6" width="21" style="6" customWidth="1"/>
+    <col min="7" max="7" width="42.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -38725,7 +38736,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>44829</v>
       </c>
@@ -38736,7 +38747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8" cm="1">
         <f t="array" aca="1" ref="A3" ca="1">_xll.EVALUATIONDATE.SET(A2)</f>
         <v>44829</v>
@@ -38748,7 +38759,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="C4" s="6" t="s">
         <v>29</v>
@@ -38757,7 +38768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C5" s="6" t="s">
         <v>30</v>
       </c>
@@ -38765,23 +38776,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="6" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">_xll.REPOSITORY.SIZE()</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="str" cm="1">
         <f t="array" aca="1" ref="A7" ca="1">_xll.PRODUCT.NEW("my_product",A17:A175,B17:B175)</f>
-        <v>~ScriptProduct~my_product~000002BAF8F0E9D0</v>
+        <v>~ScriptProduct~my_product~000002437BF38DF0</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.BSMODELDATA.NEW("model",D2,D3,D4,D5)</f>
-        <v>~BSModelData_~model~000002BA9A1C5C70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>~BSModelData_~model~000002431F97BE10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="G7" ca="1">_xll.REPOSITORY.FIND("BSModelData")</f>
+        <v>~BSModelData_~model~000002431F97BE10</v>
+      </c>
+      <c r="H7" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="H7" ca="1">_xll.REPOSITORY.FIND("ScriptProduct")</f>
+        <v>~ScriptProduct~my_product~000002437BF38DF0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="str">
         <f t="array" aca="1" ref="A10:B14" ca="1">_xll.MONTECARLO.VALUE(A7,C7,2^20,"sobol",TRUE,TRUE,0.5)</f>
         <v>d_div</v>
@@ -38792,7 +38823,7 @@
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="str">
         <f ca="1"/>
         <v>d_rate</v>
@@ -38802,7 +38833,7 @@
         <v>13.64397785215289</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="str">
         <f ca="1"/>
         <v>d_spot</v>
@@ -38812,7 +38843,7 @@
         <v>4.4502779077836147E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="str">
         <f ca="1"/>
         <v>d_vol</v>
@@ -38822,7 +38853,7 @@
         <v>-4.186599006938005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="str">
         <f ca="1"/>
         <v>value</v>
@@ -38832,7 +38863,7 @@
         <v>1.195609488594287</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>

</xml_diff>